<commit_message>
chỉnh lại giao diện login, register, làm đẹp lại giao diện
</commit_message>
<xml_diff>
--- a/_task.xlsx
+++ b/_task.xlsx
@@ -5,18 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\CodeJava\Code\React JS\BT_React\ReactJS-Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\CodeJava\Code\React JS\BT_React\test_react\ReactJS-Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7124EA83-42FA-4FD7-BEE8-B491248018DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596E17DA-1331-4665-947F-9A67347AD347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mitsg4nKYzU0T1mG+CZd0js0eHfeQ=="/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -90,9 +101,6 @@
     <t>SearchBar</t>
   </si>
   <si>
-    <t>Cinema</t>
-  </si>
-  <si>
     <t>ListCinema</t>
   </si>
   <si>
@@ -102,13 +110,58 @@
     <t>CinemaSchedule</t>
   </si>
   <si>
-    <t>Booking</t>
-  </si>
-  <si>
     <t>CurrentMovie</t>
   </si>
   <si>
     <t>ComingMovie</t>
+  </si>
+  <si>
+    <t>CinemaPage</t>
+  </si>
+  <si>
+    <t>BookingPage</t>
+  </si>
+  <si>
+    <t>BookingCinemaList</t>
+  </si>
+  <si>
+    <t>BookingMovieList</t>
+  </si>
+  <si>
+    <t>BookingScheduleList</t>
+  </si>
+  <si>
+    <t>BookingTicketPage</t>
+  </si>
+  <si>
+    <t>MovieInfo</t>
+  </si>
+  <si>
+    <t>SeatList</t>
+  </si>
+  <si>
+    <t>TotalCheckout</t>
+  </si>
+  <si>
+    <t>ManagerPage</t>
+  </si>
+  <si>
+    <t>AddMovie</t>
+  </si>
+  <si>
+    <t>HeaderHomeManager</t>
+  </si>
+  <si>
+    <t>MovieManager</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>EditProfile</t>
+  </si>
+  <si>
+    <t>EditMovie</t>
   </si>
 </sst>
 </file>
@@ -180,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -234,21 +287,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -341,11 +379,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -365,35 +466,56 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -640,12 +762,12 @@
   <dimension ref="A1:K983"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
     <col min="3" max="5" width="7.59765625" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
@@ -661,7 +783,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -693,276 +815,516 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="12"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8">
         <v>1</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="12"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8">
         <v>1</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="12"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="14" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8">
         <v>1</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="12"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="24"/>
+      <c r="B7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9">
+      <c r="B9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+      <c r="F9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9">
+      <c r="B12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8">
         <v>1</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9">
+      <c r="F12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8">
         <v>1</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8">
         <v>1</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9">
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8">
         <v>1</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9">
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8">
         <v>1</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9">
+      <c r="F16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8">
         <v>1</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9">
+      <c r="F17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8">
         <v>1</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9">
+      <c r="F18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8">
         <v>1</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="11"/>
+    </row>
+    <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8">
+        <v>1</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8">
+        <v>1</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8">
+        <v>1</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1915,17 +2277,20 @@
     <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A15:A17"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A18:A23"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E15">
+  <conditionalFormatting sqref="E2:E29">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>